<commit_message>
Calculator User Interface implementation
</commit_message>
<xml_diff>
--- a/screen metric calculations.xlsx
+++ b/screen metric calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30400" yWindow="0" windowWidth="19160" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="16900" yWindow="0" windowWidth="19160" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>calculator</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>fourth col</t>
+  </si>
+  <si>
+    <t>Calculator main buttons row coordinate calculation table</t>
+  </si>
+  <si>
+    <t>column coordinate calculation</t>
+  </si>
+  <si>
+    <t>screen size landscape</t>
+  </si>
+  <si>
+    <t>(status bar 20 poiint)</t>
+  </si>
+  <si>
+    <t>hot menu</t>
+  </si>
+  <si>
+    <t>menu (app list)</t>
+  </si>
+  <si>
+    <t>app view</t>
   </si>
 </sst>
 </file>
@@ -121,7 +142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,11 +162,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -155,6 +181,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -164,6 +191,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,197 +521,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>116</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <f>B2+D2+E2</f>
+      <c r="C4">
+        <f t="shared" ref="C4:C9" si="0">C3+E3+F3</f>
         <v>133</v>
       </c>
-      <c r="D3">
+      <c r="E4">
         <v>74</v>
       </c>
-      <c r="E3">
+      <c r="F4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <f>B3+D3+E3</f>
+      <c r="C5">
+        <f t="shared" si="0"/>
         <v>217</v>
       </c>
-      <c r="D4">
+      <c r="E5">
         <v>74</v>
       </c>
-      <c r="E4">
+      <c r="F5">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <f>B4+D4+E4</f>
+      <c r="C6">
+        <f t="shared" si="0"/>
         <v>301</v>
       </c>
-      <c r="D5">
+      <c r="E6">
         <v>74</v>
       </c>
-      <c r="E5">
+      <c r="F6">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <f>B5+D5+E5</f>
+      <c r="C7">
+        <f t="shared" si="0"/>
         <v>385</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <v>74</v>
       </c>
-      <c r="E6">
+      <c r="F7">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <f>B6+D6+E6</f>
+      <c r="C8">
+        <f t="shared" si="0"/>
         <v>469</v>
       </c>
-      <c r="D7">
+      <c r="E8">
         <v>74</v>
       </c>
-      <c r="E7">
+      <c r="F8">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <f>B7+D7+E7</f>
+      <c r="C9">
+        <f t="shared" si="0"/>
         <v>553</v>
       </c>
-      <c r="D8">
+      <c r="E9">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="B10" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="C12">
         <v>80</v>
       </c>
-      <c r="D11">
+      <c r="E12">
         <v>120</v>
       </c>
-      <c r="E11">
+      <c r="F12">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
-        <f>B11+D11+E11</f>
+      <c r="C13">
+        <f>C12+E12+F12</f>
         <v>224</v>
       </c>
-      <c r="D12">
+      <c r="E13">
         <v>120</v>
       </c>
-      <c r="E12">
+      <c r="F13">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
-        <f>B12+D12+E12</f>
+      <c r="C14">
+        <f>C13+E13+F13</f>
         <v>368</v>
       </c>
-      <c r="D13">
+      <c r="E14">
         <v>120</v>
       </c>
-      <c r="E13">
+      <c r="F14">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <f>B13+D13+E13</f>
+      <c r="C15">
+        <f>C14+E14+F14</f>
         <v>512</v>
       </c>
-      <c r="D14">
+      <c r="E15">
         <v>120</v>
       </c>
     </row>
+    <row r="16" spans="1:6">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>1024</v>
+      </c>
+      <c r="C17">
+        <v>748</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>256</v>
+      </c>
+      <c r="C19">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>714</v>
+      </c>
+      <c r="C20">
+        <v>748</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A11:A15"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
preparing for multiple contents (day, week,  month, year, list)
</commit_message>
<xml_diff>
--- a/screen metric calculations.xlsx
+++ b/screen metric calculations.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16900" yWindow="0" windowWidth="19160" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="15540" yWindow="0" windowWidth="19160" windowHeight="19020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="General" sheetId="3" r:id="rId1"/>
+    <sheet name="Calculator" sheetId="1" r:id="rId2"/>
+    <sheet name="Calendar" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>calculator</t>
   </si>
@@ -97,6 +99,24 @@
   </si>
   <si>
     <t>app Landscape full size (- hot menu width)</t>
+  </si>
+  <si>
+    <t>AppHeader</t>
+  </si>
+  <si>
+    <t>width(Landscape)</t>
+  </si>
+  <si>
+    <t>height(landscape)</t>
+  </si>
+  <si>
+    <t>height(Portrait)</t>
+  </si>
+  <si>
+    <t>App Header(navigation bar)</t>
+  </si>
+  <si>
+    <t>bottom area(today, calendar selector)</t>
   </si>
 </sst>
 </file>
@@ -145,7 +165,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,20 +187,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -191,6 +216,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -201,6 +227,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -530,10 +557,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>54</v>
+      </c>
+      <c r="C2">
+        <v>748</v>
+      </c>
+      <c r="D2">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <f>1024-54</f>
+        <v>970</v>
+      </c>
+      <c r="C3">
+        <v>44</v>
+      </c>
+      <c r="D3">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -542,7 +634,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
@@ -559,7 +651,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -574,7 +666,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -590,7 +682,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -606,7 +698,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1"/>
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -622,7 +714,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
+      <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -638,7 +730,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -654,7 +746,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -667,7 +759,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
@@ -681,7 +773,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1"/>
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -696,7 +788,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1"/>
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -712,7 +804,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="1"/>
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -728,7 +820,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="1"/>
+      <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -796,10 +888,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="45">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <f>1024-54</f>
         <v>970</v>
       </c>
@@ -817,4 +909,61 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <f>1024-54</f>
+        <v>970</v>
+      </c>
+      <c r="C2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <f>1024-54</f>
+        <v>970</v>
+      </c>
+      <c r="C3" s="4">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>